<commit_message>
Correzioni richieste ai file report-checklist.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#TS23XX/TS23/TServe/V.1.4.46.0/accreditamento-checklist_V8.2.7.xlsx
+++ b/GATEWAY/A1#111#TS23XX/TS23/TServe/V.1.4.46.0/accreditamento-checklist_V8.2.7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\windows\Desktop\TServe\Accreditamento bis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96565C99-1F6B-4012-B519-6F3A35B31C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E194A64D-1DCF-4739-82CD-75A4FF7C5413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="270" yWindow="3645" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Summary!$A$1:$G$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$W$190</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$W$193</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="445">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -3797,13 +3797,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W750"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B184" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="P184" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5:D5"/>
+      <selection pane="bottomRight" activeCell="S184" sqref="S184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4088,7 +4089,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33">
         <v>4</v>
       </c>
@@ -4125,7 +4126,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="35">
         <v>28</v>
       </c>
@@ -4162,7 +4163,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="35">
         <v>29</v>
       </c>
@@ -4236,7 +4237,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35">
         <v>31</v>
       </c>
@@ -4273,7 +4274,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35">
         <v>32</v>
       </c>
@@ -4310,7 +4311,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="35">
         <v>33</v>
       </c>
@@ -4347,7 +4348,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="35">
         <v>34</v>
       </c>
@@ -4384,7 +4385,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="35">
         <v>35</v>
       </c>
@@ -4421,7 +4422,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="35">
         <v>36</v>
       </c>
@@ -4458,7 +4459,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="35">
         <v>37</v>
       </c>
@@ -4532,7 +4533,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="35">
         <v>39</v>
       </c>
@@ -4569,7 +4570,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="35">
         <v>40</v>
       </c>
@@ -4606,7 +4607,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="35">
         <v>41</v>
       </c>
@@ -4643,7 +4644,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="35">
         <v>42</v>
       </c>
@@ -4680,7 +4681,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="35">
         <v>43</v>
       </c>
@@ -4717,7 +4718,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="35">
         <v>44</v>
       </c>
@@ -4756,7 +4757,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="35">
         <v>45</v>
       </c>
@@ -4834,7 +4835,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="35">
         <v>47</v>
       </c>
@@ -4873,7 +4874,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="35">
         <v>48</v>
       </c>
@@ -4912,7 +4913,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="35">
         <v>49</v>
       </c>
@@ -4951,7 +4952,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="35">
         <v>50</v>
       </c>
@@ -4990,7 +4991,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="35">
         <v>51</v>
       </c>
@@ -5029,7 +5030,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="35">
         <v>53</v>
       </c>
@@ -5066,7 +5067,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="35">
         <v>55</v>
       </c>
@@ -5103,7 +5104,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="35">
         <v>56</v>
       </c>
@@ -5140,7 +5141,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="35">
         <v>57</v>
       </c>
@@ -5177,7 +5178,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="35">
         <v>59</v>
       </c>
@@ -5214,7 +5215,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="35">
         <v>60</v>
       </c>
@@ -5251,7 +5252,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="35">
         <v>61</v>
       </c>
@@ -5288,7 +5289,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="35">
         <v>62</v>
       </c>
@@ -5325,7 +5326,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="35">
         <v>64</v>
       </c>
@@ -5362,7 +5363,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="35">
         <v>66</v>
       </c>
@@ -5399,7 +5400,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35">
         <v>67</v>
       </c>
@@ -5436,7 +5437,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="35">
         <v>68</v>
       </c>
@@ -5473,7 +5474,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="35">
         <v>69</v>
       </c>
@@ -5510,7 +5511,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="35">
         <v>70</v>
       </c>
@@ -5547,7 +5548,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="35">
         <v>71</v>
       </c>
@@ -5584,7 +5585,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="35">
         <v>72</v>
       </c>
@@ -5621,7 +5622,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="35">
         <v>73</v>
       </c>
@@ -5658,7 +5659,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="35">
         <v>74</v>
       </c>
@@ -5695,7 +5696,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="35">
         <v>76</v>
       </c>
@@ -5732,7 +5733,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="35">
         <v>78</v>
       </c>
@@ -5769,7 +5770,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="35">
         <v>79</v>
       </c>
@@ -5806,7 +5807,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="35">
         <v>80</v>
       </c>
@@ -5843,7 +5844,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="35">
         <v>81</v>
       </c>
@@ -5880,7 +5881,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="35">
         <v>83</v>
       </c>
@@ -5917,7 +5918,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="35">
         <v>84</v>
       </c>
@@ -5954,7 +5955,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="35">
         <v>85</v>
       </c>
@@ -5991,7 +5992,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="35">
         <v>86</v>
       </c>
@@ -6028,7 +6029,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="35">
         <v>87</v>
       </c>
@@ -6065,7 +6066,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="35">
         <v>88</v>
       </c>
@@ -6102,7 +6103,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="35">
         <v>89</v>
       </c>
@@ -6139,7 +6140,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="35">
         <v>90</v>
       </c>
@@ -6176,7 +6177,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="35">
         <v>91</v>
       </c>
@@ -6213,7 +6214,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="35">
         <v>92</v>
       </c>
@@ -6250,7 +6251,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="35">
         <v>93</v>
       </c>
@@ -6287,7 +6288,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="35">
         <v>95</v>
       </c>
@@ -6324,7 +6325,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="35">
         <v>97</v>
       </c>
@@ -6361,7 +6362,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="71" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="35">
         <v>98</v>
       </c>
@@ -6398,7 +6399,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="35">
         <v>99</v>
       </c>
@@ -6435,7 +6436,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="35">
         <v>100</v>
       </c>
@@ -6472,7 +6473,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="35">
         <v>101</v>
       </c>
@@ -6509,7 +6510,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="35">
         <v>102</v>
       </c>
@@ -6546,7 +6547,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="35">
         <v>103</v>
       </c>
@@ -6583,7 +6584,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="35">
         <v>104</v>
       </c>
@@ -6620,7 +6621,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="35">
         <v>105</v>
       </c>
@@ -6657,7 +6658,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="79" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="35">
         <v>106</v>
       </c>
@@ -6694,7 +6695,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="35">
         <v>108</v>
       </c>
@@ -6731,7 +6732,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="81" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="35">
         <v>110</v>
       </c>
@@ -6768,7 +6769,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="35">
         <v>111</v>
       </c>
@@ -6805,7 +6806,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="83" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="35">
         <v>112</v>
       </c>
@@ -6842,7 +6843,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="35">
         <v>113</v>
       </c>
@@ -6879,7 +6880,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="35">
         <v>114</v>
       </c>
@@ -6916,7 +6917,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="35">
         <v>115</v>
       </c>
@@ -6953,7 +6954,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="87" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="35">
         <v>116</v>
       </c>
@@ -6990,7 +6991,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="35">
         <v>117</v>
       </c>
@@ -7027,7 +7028,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="35">
         <v>118</v>
       </c>
@@ -7064,7 +7065,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="35">
         <v>119</v>
       </c>
@@ -7101,7 +7102,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="91" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="35">
         <v>120</v>
       </c>
@@ -7138,7 +7139,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="92" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="35">
         <v>121</v>
       </c>
@@ -7175,7 +7176,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="35">
         <v>123</v>
       </c>
@@ -7212,7 +7213,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="94" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="35">
         <v>125</v>
       </c>
@@ -7249,7 +7250,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="35">
         <v>126</v>
       </c>
@@ -7286,7 +7287,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="35">
         <v>127</v>
       </c>
@@ -7323,7 +7324,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="97" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="35">
         <v>128</v>
       </c>
@@ -7360,7 +7361,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="98" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="35">
         <v>129</v>
       </c>
@@ -7397,7 +7398,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="99" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="35">
         <v>130</v>
       </c>
@@ -7434,7 +7435,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="35">
         <v>131</v>
       </c>
@@ -7471,7 +7472,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="101" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="35">
         <v>132</v>
       </c>
@@ -7508,7 +7509,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="102" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="35">
         <v>133</v>
       </c>
@@ -7545,7 +7546,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="35">
         <v>134</v>
       </c>
@@ -7582,7 +7583,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="104" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="35">
         <v>135</v>
       </c>
@@ -7619,7 +7620,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="105" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="35">
         <v>136</v>
       </c>
@@ -7656,7 +7657,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="106" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="35">
         <v>137</v>
       </c>
@@ -7693,7 +7694,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="35">
         <v>138</v>
       </c>
@@ -7730,7 +7731,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="108" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="35">
         <v>139</v>
       </c>
@@ -7767,7 +7768,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="109" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="35">
         <v>140</v>
       </c>
@@ -7804,7 +7805,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="35">
         <v>141</v>
       </c>
@@ -7841,7 +7842,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="111" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="35">
         <v>142</v>
       </c>
@@ -7878,7 +7879,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="112" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="35">
         <v>143</v>
       </c>
@@ -7915,7 +7916,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="113" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="35">
         <v>144</v>
       </c>
@@ -7952,7 +7953,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="114" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="35">
         <v>145</v>
       </c>
@@ -7989,7 +7990,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="115" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="35">
         <v>146</v>
       </c>
@@ -8026,7 +8027,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="116" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="35">
         <v>152</v>
       </c>
@@ -8063,7 +8064,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="117" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="35">
         <v>154</v>
       </c>
@@ -8100,7 +8101,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="118" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="35">
         <v>155</v>
       </c>
@@ -8137,7 +8138,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="119" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="35">
         <v>156</v>
       </c>
@@ -8174,7 +8175,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="120" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="35">
         <v>159</v>
       </c>
@@ -8211,7 +8212,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="121" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="35">
         <v>160</v>
       </c>
@@ -8248,7 +8249,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="122" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="35">
         <v>161</v>
       </c>
@@ -8285,7 +8286,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="35">
         <v>162</v>
       </c>
@@ -8322,7 +8323,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="35">
         <v>163</v>
       </c>
@@ -8359,7 +8360,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="125" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="35">
         <v>164</v>
       </c>
@@ -8396,7 +8397,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="126" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="35">
         <v>165</v>
       </c>
@@ -8433,7 +8434,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="127" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="35">
         <v>166</v>
       </c>
@@ -8470,7 +8471,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="35">
         <v>167</v>
       </c>
@@ -8507,7 +8508,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="129" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="35">
         <v>168</v>
       </c>
@@ -8544,7 +8545,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="130" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="35">
         <v>169</v>
       </c>
@@ -9136,7 +9137,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="146" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="35">
         <v>191</v>
       </c>
@@ -9173,7 +9174,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="147" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="35">
         <v>376</v>
       </c>
@@ -9210,7 +9211,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="148" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="35">
         <v>417</v>
       </c>
@@ -9247,7 +9248,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="149" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="35">
         <v>418</v>
       </c>
@@ -9284,7 +9285,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="150" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="35">
         <v>419</v>
       </c>
@@ -9321,7 +9322,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="151" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="35">
         <v>423</v>
       </c>
@@ -9358,7 +9359,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="152" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="35">
         <v>424</v>
       </c>
@@ -9395,7 +9396,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="153" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="35">
         <v>425</v>
       </c>
@@ -9432,7 +9433,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="154" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="35">
         <v>432</v>
       </c>
@@ -9469,7 +9470,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="155" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="35">
         <v>433</v>
       </c>
@@ -9506,7 +9507,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="156" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="35">
         <v>434</v>
       </c>
@@ -9543,7 +9544,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="157" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="35">
         <v>435</v>
       </c>
@@ -9580,7 +9581,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="158" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="35">
         <v>437</v>
       </c>
@@ -9617,7 +9618,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="159" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="35">
         <v>438</v>
       </c>
@@ -9654,7 +9655,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="160" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="35">
         <v>440</v>
       </c>
@@ -9691,7 +9692,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="161" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="35">
         <v>441</v>
       </c>
@@ -9728,7 +9729,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="162" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="35">
         <v>442</v>
       </c>
@@ -9765,7 +9766,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="163" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="35">
         <v>443</v>
       </c>
@@ -9802,7 +9803,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="164" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="35">
         <v>448</v>
       </c>
@@ -9839,7 +9840,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="165" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="35">
         <v>449</v>
       </c>
@@ -9876,7 +9877,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="166" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="35">
         <v>450</v>
       </c>
@@ -9913,7 +9914,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="167" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="35">
         <v>451</v>
       </c>
@@ -9950,7 +9951,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="168" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="35">
         <v>452</v>
       </c>
@@ -9987,7 +9988,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="35">
         <v>454</v>
       </c>
@@ -10024,7 +10025,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="170" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="35">
         <v>455</v>
       </c>
@@ -10061,7 +10062,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="171" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="35">
         <v>456</v>
       </c>
@@ -10098,7 +10099,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="172" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="35">
         <v>457</v>
       </c>
@@ -10135,7 +10136,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="173" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="35">
         <v>458</v>
       </c>
@@ -10172,7 +10173,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="174" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="35">
         <v>459</v>
       </c>
@@ -10209,7 +10210,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="175" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="35">
         <v>460</v>
       </c>
@@ -10246,7 +10247,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="176" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="35">
         <v>461</v>
       </c>
@@ -10283,7 +10284,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="177" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="35">
         <v>462</v>
       </c>
@@ -10320,7 +10321,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="178" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="35">
         <v>463</v>
       </c>
@@ -10357,7 +10358,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="179" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="35">
         <v>464</v>
       </c>
@@ -10394,7 +10395,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="180" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="35">
         <v>465</v>
       </c>
@@ -10431,7 +10432,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="181" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="35">
         <v>466</v>
       </c>
@@ -10468,7 +10469,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="182" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="35">
         <v>467</v>
       </c>
@@ -10505,7 +10506,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="183" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="35">
         <v>468</v>
       </c>
@@ -10562,7 +10563,9 @@
       <c r="G184" s="35"/>
       <c r="H184" s="35"/>
       <c r="I184" s="35"/>
-      <c r="J184" s="38"/>
+      <c r="J184" s="38" t="s">
+        <v>64</v>
+      </c>
       <c r="K184" s="38"/>
       <c r="L184" s="35"/>
       <c r="M184" s="38"/>
@@ -10579,7 +10582,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="185" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="35">
         <v>470</v>
       </c>
@@ -10616,7 +10619,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="186" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="35">
         <v>471</v>
       </c>
@@ -10653,7 +10656,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="187" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="35">
         <v>472</v>
       </c>
@@ -10690,7 +10693,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="188" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="35">
         <v>473</v>
       </c>
@@ -10727,7 +10730,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="189" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="35">
         <v>474</v>
       </c>
@@ -10764,7 +10767,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="190" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="35">
         <v>475</v>
       </c>
@@ -10821,7 +10824,9 @@
       <c r="G191" s="37"/>
       <c r="H191" s="37"/>
       <c r="I191" s="42"/>
-      <c r="J191" s="38"/>
+      <c r="J191" s="38" t="s">
+        <v>64</v>
+      </c>
       <c r="K191" s="38"/>
       <c r="L191" s="38"/>
       <c r="M191" s="38"/>
@@ -10858,7 +10863,9 @@
       <c r="G192" s="37"/>
       <c r="H192" s="37"/>
       <c r="I192" s="42"/>
-      <c r="J192" s="38"/>
+      <c r="J192" s="38" t="s">
+        <v>64</v>
+      </c>
       <c r="K192" s="38"/>
       <c r="L192" s="38"/>
       <c r="M192" s="38"/>
@@ -14879,7 +14886,13 @@
     <row r="749" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="750" spans="23:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A9:W190" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
+  <autoFilter ref="A9:W193" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="PSS"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>

</xml_diff>